<commit_message>
Classificazione a tre variabili
</commit_message>
<xml_diff>
--- a/Excel/RandomForest_Results.xlsx
+++ b/Excel/RandomForest_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabry\OneDrive\Documenti\GitHub\AnalisiDatasetDiabete\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596418EE-2507-4D89-A820-BB7A062AD021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81620C99-EF11-451C-B739-CDBFE427D375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1236" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1392" yWindow="1584" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice&amp;Risultati" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="BQ2">
         <f>SUM(Split_80_20!D2:G2)</f>
-        <v>2.9447775029608732</v>
+        <v>2.944777502960874</v>
       </c>
       <c r="BR2">
         <f>SUM(KFold_CV!E2:H2)</f>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="BT4">
         <f>SUM(Split_80_20_Test!D4:G4)</f>
-        <v>2.7935187320039252</v>
+        <v>2.7935187320039261</v>
       </c>
       <c r="BU4">
         <f>SUM(KFold_CV_Test!E4:H4)</f>
@@ -2371,7 +2371,7 @@
     <row r="6" spans="1:75" x14ac:dyDescent="0.3">
       <c r="BQ6">
         <f>SUM(Split_80_20!D6:G6)</f>
-        <v>2.9132643249204198</v>
+        <v>2.9132643249204202</v>
       </c>
       <c r="BR6">
         <f>SUM(KFold_CV!E6:H6)</f>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="BT7">
         <f>SUM(Split_80_20_Test!D7:G7)</f>
-        <v>2.8711494252873564</v>
+        <v>2.8711494252873573</v>
       </c>
       <c r="BU7">
         <f>SUM(KFold_CV_Test!E7:H7)</f>
@@ -2540,7 +2540,7 @@
       <c r="F10" s="5"/>
       <c r="BQ10">
         <f>SUM(Split_80_20!D10:G10)</f>
-        <v>2.8853541966826137</v>
+        <v>2.8853541966826142</v>
       </c>
       <c r="BR10">
         <f>SUM(KFold_CV!E10:H10)</f>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="BW12">
         <f>SUM(Split_80_20_Test!D12:G12)</f>
-        <v>2.8579209411551858</v>
+        <v>2.8579209411551871</v>
       </c>
     </row>
     <row r="13" spans="1:75" x14ac:dyDescent="0.3">
@@ -2740,7 +2740,7 @@
       <c r="F16" s="20"/>
       <c r="BQ16">
         <f>SUM(Split_80_20!D16:G16)</f>
-        <v>2.8309131480771241</v>
+        <v>2.8309131480771246</v>
       </c>
       <c r="BR16">
         <f>SUM(KFold_CV!E16:H16)</f>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="BW17">
         <f>SUM(Split_80_20_Test!D17:G17)</f>
-        <v>2.8853541966826137</v>
+        <v>2.8853541966826142</v>
       </c>
     </row>
     <row r="18" spans="1:78" x14ac:dyDescent="0.3">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="BZ18">
         <f>SUM(Split_80_20_Test!D18:G18)</f>
-        <v>2.8447783588202769</v>
+        <v>2.8447783588202782</v>
       </c>
     </row>
     <row r="19" spans="1:78" x14ac:dyDescent="0.3">
@@ -2934,7 +2934,7 @@
       <c r="F21" s="20"/>
       <c r="BQ21">
         <f>SUM(Split_80_20!D21:G21)</f>
-        <v>2.8309131480771241</v>
+        <v>2.8309131480771246</v>
       </c>
       <c r="BR21">
         <f>SUM(KFold_CV!E21:H21)</f>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="BZ22">
         <f>SUM(Split_80_20_Test!D22:G22)</f>
-        <v>2.8741399483822683</v>
+        <v>2.8741399483822692</v>
       </c>
     </row>
     <row r="23" spans="1:78" x14ac:dyDescent="0.3">
@@ -3424,7 +3424,7 @@
       </c>
       <c r="B37" s="6">
         <f>MAX(BQ:BQ)</f>
-        <v>2.9447775029608732</v>
+        <v>2.944777502960874</v>
       </c>
       <c r="C37" s="6">
         <f>MAX(BR:BR)</f>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B38" s="6">
         <f>MAX(BT:BT, BW:BW, BZ:BZ)</f>
-        <v>2.8853541966826137</v>
+        <v>2.8853541966826142</v>
       </c>
       <c r="C38" s="6">
         <f>MAX(BU:BU, BX:BX, CA:CA)</f>
@@ -4856,7 +4856,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BQ1" sqref="BQ1:BQ1048576"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4965,13 +4965,13 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>0.7448275862068966</v>
+        <v>0.74482758620689704</v>
       </c>
       <c r="E2">
-        <v>0.73001136794240251</v>
+        <v>0.73001136794240296</v>
       </c>
       <c r="F2">
-        <v>0.7448275862068966</v>
+        <v>0.74482758620689704</v>
       </c>
       <c r="G2">
         <v>0.725110962604677</v>
@@ -5321,16 +5321,16 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.73793103448275865</v>
+        <v>0.73793103448275899</v>
       </c>
       <c r="E6">
-        <v>0.72141048120007789</v>
+        <v>0.721410481200078</v>
       </c>
       <c r="F6">
-        <v>0.73793103448275865</v>
+        <v>0.73793103448275899</v>
       </c>
       <c r="G6">
-        <v>0.71599177475482445</v>
+        <v>0.71599177475482401</v>
       </c>
       <c r="H6" t="s">
         <v>66</v>
@@ -5677,16 +5677,16 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="E10">
-        <v>0.71303313544692859</v>
+        <v>0.71303313544692903</v>
       </c>
       <c r="F10">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="G10">
-        <v>0.71025209571844339</v>
+        <v>0.71025209571844306</v>
       </c>
       <c r="H10" t="s">
         <v>70</v>
@@ -6211,16 +6211,16 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>0.71724137931034482</v>
+        <v>0.71724137931034504</v>
       </c>
       <c r="E16">
-        <v>0.69760119940029974</v>
+        <v>0.69760119940029996</v>
       </c>
       <c r="F16">
-        <v>0.71724137931034482</v>
+        <v>0.71724137931034504</v>
       </c>
       <c r="G16">
-        <v>0.69882919005613464</v>
+        <v>0.69882919005613497</v>
       </c>
       <c r="H16" t="s">
         <v>73</v>
@@ -6656,16 +6656,16 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <v>0.71724137931034482</v>
+        <v>0.71724137931034504</v>
       </c>
       <c r="E21">
-        <v>0.69760119940029974</v>
+        <v>0.69760119940029996</v>
       </c>
       <c r="F21">
-        <v>0.71724137931034482</v>
+        <v>0.71724137931034504</v>
       </c>
       <c r="G21">
-        <v>0.69882919005613464</v>
+        <v>0.69882919005613497</v>
       </c>
       <c r="H21" t="s">
         <v>73</v>
@@ -16053,7 +16053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -25362,8 +25362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BG25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:BG25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25734,16 +25734,16 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0.71034482758620687</v>
+        <v>0.71034482758620698</v>
       </c>
       <c r="E4">
-        <v>0.68673290473407367</v>
+        <v>0.686732904734074</v>
       </c>
       <c r="F4">
-        <v>0.71034482758620687</v>
+        <v>0.71034482758620698</v>
       </c>
       <c r="G4">
-        <v>0.68609617209743756</v>
+        <v>0.68609617209743801</v>
       </c>
       <c r="H4" t="s">
         <v>75</v>
@@ -26001,16 +26001,16 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="E7">
-        <v>0.71482758620689657</v>
+        <v>0.71482758620689701</v>
       </c>
       <c r="F7">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="G7">
-        <v>0.69425287356321841</v>
+        <v>0.69425287356321796</v>
       </c>
       <c r="H7" t="s">
         <v>236</v>
@@ -26446,16 +26446,16 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0.72413793103448276</v>
+        <v>0.72413793103448298</v>
       </c>
       <c r="E12">
-        <v>0.70511296076099883</v>
+        <v>0.70511296076099905</v>
       </c>
       <c r="F12">
-        <v>0.72413793103448276</v>
+        <v>0.72413793103448298</v>
       </c>
       <c r="G12">
-        <v>0.70453211832522178</v>
+        <v>0.704532118325222</v>
       </c>
       <c r="H12" t="s">
         <v>187</v>
@@ -26891,16 +26891,16 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="E17">
-        <v>0.71303313544692859</v>
+        <v>0.71303313544692903</v>
       </c>
       <c r="F17">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="G17">
-        <v>0.71025209571844339</v>
+        <v>0.71025209571844306</v>
       </c>
       <c r="H17" t="s">
         <v>70</v>
@@ -26980,16 +26980,16 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>0.72413793103448276</v>
+        <v>0.72413793103448298</v>
       </c>
       <c r="E18">
-        <v>0.70332047091208494</v>
+        <v>0.70332047091208505</v>
       </c>
       <c r="F18">
-        <v>0.72413793103448276</v>
+        <v>0.72413793103448298</v>
       </c>
       <c r="G18">
-        <v>0.69318202583922661</v>
+        <v>0.69318202583922695</v>
       </c>
       <c r="H18" t="s">
         <v>237</v>
@@ -27504,16 +27504,16 @@
         <v>5</v>
       </c>
       <c r="D22">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="E22">
-        <v>0.71333180416443664</v>
+        <v>0.71333180416443698</v>
       </c>
       <c r="F22">
-        <v>0.73103448275862071</v>
+        <v>0.73103448275862104</v>
       </c>
       <c r="G22">
-        <v>0.69873917870059021</v>
+        <v>0.69873917870058999</v>
       </c>
       <c r="H22" t="s">
         <v>238</v>
@@ -40941,7 +40941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BH121"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>

</xml_diff>